<commit_message>
Archive_copy + clean up FRD4P + Start up FRI4P
</commit_message>
<xml_diff>
--- a/FRD4P/Test/FRD4P_df.xlsx
+++ b/FRD4P/Test/FRD4P_df.xlsx
@@ -8,13 +8,16 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/FRD4P/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="2" documentId="11_6F7DF2A6D300DB58BF183311595ED87656CD4FAC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{600BE445-898C-43A8-8603-F66ACCAD0927}"/>
+  <xr:revisionPtr revIDLastSave="4" documentId="11_6F7DF2A6D3C05237A31B3611595ED87656CD4FAC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC18FCA2-8DCF-4510-B0FC-6688B7E3898E}"/>
   <bookViews>
-    <workbookView xWindow="-315" yWindow="-16320" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
+  <definedNames>
+    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$41</definedName>
+  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -719,12 +722,11 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:H41"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0"/>
+    <sheetView tabSelected="1" workbookViewId="0">
+      <selection activeCell="H2" sqref="H2"/>
+    </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
-  <cols>
-    <col min="7" max="7" width="23.140625" bestFit="1" customWidth="1"/>
-  </cols>
   <sheetData>
     <row r="1" spans="1:8" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">

</xml_diff>

<commit_message>
12122024 setup modularity for index reviews
</commit_message>
<xml_diff>
--- a/FRD4P/Test/FRD4P_df.xlsx
+++ b/FRD4P/Test/FRD4P_df.xlsx
@@ -8,16 +8,13 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://euronext-my.sharepoint.com/personal/csonneveld_euronext_com/Documents/Documents/Projects/FRD4P/Test/"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="4" documentId="11_6F7DF2A6D3C05237A31B3611595ED87656CD4FAC" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{AC18FCA2-8DCF-4510-B0FC-6688B7E3898E}"/>
+  <xr:revisionPtr revIDLastSave="15" documentId="11_4D9972A1D320D417777B3211595ED87656CD7F26" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{2644A60B-3A83-40DC-B8E9-BD59C09EBD79}"/>
   <bookViews>
-    <workbookView xWindow="-29115" yWindow="-16005" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-29370" yWindow="195" windowWidth="29040" windowHeight="15840" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <definedNames>
-    <definedName name="_xlnm._FilterDatabase" localSheetId="0" hidden="1">Sheet1!$A$1:$H$41</definedName>
-  </definedNames>
   <calcPr calcId="191029"/>
   <extLst>
     <ext xmlns:xcalcf="http://schemas.microsoft.com/office/spreadsheetml/2018/calcfeatures" uri="{B58B0392-4F1F-4190-BB64-5DF3571DCE5F}">
@@ -36,7 +33,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="208" uniqueCount="107">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="308" uniqueCount="109">
   <si>
     <t>Name</t>
   </si>
@@ -71,7 +68,7 @@
     <t>XLON</t>
   </si>
   <si>
-    <t>23-Sep-24</t>
+    <t>23-Dec-24</t>
   </si>
   <si>
     <t>GBP</t>
@@ -101,6 +98,18 @@
     <t>EUR</t>
   </si>
   <si>
+    <t>ADMIRAL GROUP PLC</t>
+  </si>
+  <si>
+    <t>GB00B02J6398</t>
+  </si>
+  <si>
+    <t>ALSTOM</t>
+  </si>
+  <si>
+    <t>FR0010220475</t>
+  </si>
+  <si>
     <t>AMADEUS IT GROUP</t>
   </si>
   <si>
@@ -110,16 +119,10 @@
     <t>XMAD</t>
   </si>
   <si>
-    <t>AMCOR PLC</t>
-  </si>
-  <si>
-    <t>JE00BJ1F3079</t>
-  </si>
-  <si>
-    <t>ARKEMA</t>
-  </si>
-  <si>
-    <t>FR0010313833</t>
+    <t>ASTRAZENECA</t>
+  </si>
+  <si>
+    <t>GB0009895292</t>
   </si>
   <si>
     <t>AXA</t>
@@ -128,6 +131,27 @@
     <t>FR0000120628</t>
   </si>
   <si>
+    <t>BECTON DICKINSON</t>
+  </si>
+  <si>
+    <t>US0758871091</t>
+  </si>
+  <si>
+    <t>BIOGEN INC</t>
+  </si>
+  <si>
+    <t>US09062X1037</t>
+  </si>
+  <si>
+    <t>XNGS</t>
+  </si>
+  <si>
+    <t>BIOMERIEUX</t>
+  </si>
+  <si>
+    <t>FR0013280286</t>
+  </si>
+  <si>
     <t>BLACKSTONE INC</t>
   </si>
   <si>
@@ -140,16 +164,10 @@
     <t>FR0000131104</t>
   </si>
   <si>
-    <t>BUREAU VERITAS</t>
-  </si>
-  <si>
-    <t>FR0006174348</t>
-  </si>
-  <si>
-    <t>CARREFOUR</t>
-  </si>
-  <si>
-    <t>FR0000120172</t>
+    <t>BOUYGUES</t>
+  </si>
+  <si>
+    <t>FR0000120503</t>
   </si>
   <si>
     <t>CGI INC. CLASS A</t>
@@ -194,9 +212,6 @@
     <t>US29444U7000</t>
   </si>
   <si>
-    <t>XNGS</t>
-  </si>
-  <si>
     <t>GENERAL MILLS INC.</t>
   </si>
   <si>
@@ -215,12 +230,6 @@
     <t>FR0000052292</t>
   </si>
   <si>
-    <t>KERING</t>
-  </si>
-  <si>
-    <t>FR0000121485</t>
-  </si>
-  <si>
     <t>KINGFISHER</t>
   </si>
   <si>
@@ -248,34 +257,19 @@
     <t>XETR</t>
   </si>
   <si>
-    <t>MICHELIN</t>
-  </si>
-  <si>
-    <t>FR001400AJ45</t>
-  </si>
-  <si>
-    <t>NESTLE SA</t>
-  </si>
-  <si>
-    <t>CH0038863350</t>
-  </si>
-  <si>
-    <t>XSWX</t>
-  </si>
-  <si>
-    <t>CHF</t>
-  </si>
-  <si>
     <t>NEXANS</t>
   </si>
   <si>
     <t>FR0000044448</t>
   </si>
   <si>
-    <t>PERNOD RICARD</t>
-  </si>
-  <si>
-    <t>FR0000120693</t>
+    <t>NOKIA</t>
+  </si>
+  <si>
+    <t>FI0009000681</t>
+  </si>
+  <si>
+    <t>XHEL</t>
   </si>
   <si>
     <t>PUBLICIS GROUPE SA</t>
@@ -293,6 +287,12 @@
     <t>XAMS</t>
   </si>
   <si>
+    <t>RENAULT</t>
+  </si>
+  <si>
+    <t>FR0000131906</t>
+  </si>
+  <si>
     <t>REXEL</t>
   </si>
   <si>
@@ -305,16 +305,10 @@
     <t>FR0000125007</t>
   </si>
   <si>
-    <t>SECURITAS AB</t>
-  </si>
-  <si>
-    <t>SE0000163594</t>
-  </si>
-  <si>
-    <t>XSTO</t>
-  </si>
-  <si>
-    <t>SEK</t>
+    <t>SANOFI</t>
+  </si>
+  <si>
+    <t>FR0000120578</t>
   </si>
   <si>
     <t>SIEMENS AG</t>
@@ -323,10 +317,10 @@
     <t>DE0007236101</t>
   </si>
   <si>
-    <t>SWISS LIFE HOLDING</t>
-  </si>
-  <si>
-    <t>CH0014852781</t>
+    <t>STMICROELECTRONICS</t>
+  </si>
+  <si>
+    <t>NL0000226223</t>
   </si>
   <si>
     <t>THERMO FISHER SCIENT</t>
@@ -353,17 +347,29 @@
     <t>FR0000125486</t>
   </si>
   <si>
-    <t>ZIMMER BIOMET HOLD.</t>
-  </si>
-  <si>
-    <t>US98956P1021</t>
+    <t>FR0014000MR3</t>
+  </si>
+  <si>
+    <t>US6092071058</t>
+  </si>
+  <si>
+    <t/>
+  </si>
+  <si>
+    <t>EUROFINS SCIENT.</t>
+  </si>
+  <si>
+    <t>MONDELEZ INT CLASS A</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
 <styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
-  <fonts count="2" x14ac:knownFonts="1">
+  <numFmts count="1">
+    <numFmt numFmtId="43" formatCode="_(* #,##0.00_);_(* \(#,##0.00\);_(* &quot;-&quot;??_);_(@_)"/>
+  </numFmts>
+  <fonts count="4" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
       <color theme="1"/>
@@ -377,16 +383,42 @@
       <name val="Calibri"/>
       <family val="2"/>
     </font>
+    <font>
+      <sz val="11"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
+    <font>
+      <sz val="8"/>
+      <color theme="1"/>
+      <name val="Calibri"/>
+      <family val="2"/>
+      <scheme val="minor"/>
+    </font>
   </fonts>
-  <fills count="2">
+  <fills count="4">
     <fill>
       <patternFill patternType="none"/>
     </fill>
     <fill>
       <patternFill patternType="gray125"/>
     </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor theme="4" tint="0.79998168889431442"/>
+        <bgColor theme="4" tint="0.79998168889431442"/>
+      </patternFill>
+    </fill>
+    <fill>
+      <patternFill patternType="solid">
+        <fgColor rgb="FFFFFF00"/>
+        <bgColor indexed="64"/>
+      </patternFill>
+    </fill>
   </fills>
-  <borders count="2">
+  <borders count="3">
     <border>
       <left/>
       <right/>
@@ -409,20 +441,51 @@
       </bottom>
       <diagonal/>
     </border>
+    <border>
+      <left/>
+      <right/>
+      <top style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </top>
+      <bottom style="thin">
+        <color theme="4" tint="0.39997558519241921"/>
+      </bottom>
+      <diagonal/>
+    </border>
   </borders>
-  <cellStyleXfs count="1">
+  <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
+    <xf numFmtId="43" fontId="2" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="2">
+  <cellXfs count="5">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
     <xf numFmtId="0" fontId="1" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="top"/>
     </xf>
+    <xf numFmtId="43" fontId="3" fillId="2" borderId="2" xfId="1" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="43" fontId="3" fillId="0" borderId="2" xfId="1" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="0" fillId="3" borderId="0" xfId="0" applyFill="1"/>
   </cellXfs>
-  <cellStyles count="1">
+  <cellStyles count="2">
+    <cellStyle name="Comma" xfId="1" builtinId="3"/>
     <cellStyle name="Normal" xfId="0" builtinId="0"/>
   </cellStyles>
-  <dxfs count="0"/>
+  <dxfs count="2">
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+    <dxf>
+      <fill>
+        <patternFill>
+          <bgColor rgb="FFFFFF00"/>
+        </patternFill>
+      </fill>
+    </dxf>
+  </dxfs>
   <tableStyles count="0" defaultTableStyle="TableStyleMedium9" defaultPivotStyle="PivotStyleLight16"/>
   <extLst>
     <ext xmlns:x14="http://schemas.microsoft.com/office/spreadsheetml/2009/9/main" uri="{EB79DEF2-80B8-43e5-95BD-54CBDDF9020C}">
@@ -720,15 +783,15 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:H41"/>
+  <dimension ref="A1:K51"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="H2" sqref="H2"/>
+      <selection activeCell="F2" sqref="F2"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="15" x14ac:dyDescent="0.25"/>
   <sheetData>
-    <row r="1" spans="1:8" x14ac:dyDescent="0.25">
+    <row r="1" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -754,8 +817,8 @@
         <v>7</v>
       </c>
     </row>
-    <row r="2" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A2" t="s">
+    <row r="2" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A2" s="4" t="s">
         <v>8</v>
       </c>
       <c r="B2" t="s">
@@ -765,13 +828,13 @@
         <v>10</v>
       </c>
       <c r="D2">
-        <v>973383700</v>
+        <v>973388700</v>
       </c>
       <c r="E2">
         <v>1</v>
       </c>
       <c r="F2">
-        <v>0.49351445259803001</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G2" t="s">
         <v>11</v>
@@ -779,9 +842,19 @@
       <c r="H2" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="3" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A3" t="s">
+      <c r="I2" s="2" t="s">
+        <v>8</v>
+      </c>
+      <c r="J2" s="2" t="s">
+        <v>9</v>
+      </c>
+      <c r="K2" t="b">
+        <f>I2=A2</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="3" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A3" s="4" t="s">
         <v>13</v>
       </c>
       <c r="B3" t="s">
@@ -791,13 +864,13 @@
         <v>15</v>
       </c>
       <c r="D3">
-        <v>626384400</v>
+        <v>624855650</v>
       </c>
       <c r="E3">
         <v>1</v>
       </c>
       <c r="F3">
-        <v>0.49351445259803001</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G3" t="s">
         <v>11</v>
@@ -805,9 +878,19 @@
       <c r="H3" t="s">
         <v>16</v>
       </c>
-    </row>
-    <row r="4" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A4" t="s">
+      <c r="I3" s="3" t="s">
+        <v>13</v>
+      </c>
+      <c r="J3" s="3" t="s">
+        <v>14</v>
+      </c>
+      <c r="K3" t="b">
+        <f t="shared" ref="K3:K49" si="0">I3=A3</f>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="4" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A4" s="4" t="s">
         <v>17</v>
       </c>
       <c r="B4" t="s">
@@ -817,7 +900,7 @@
         <v>19</v>
       </c>
       <c r="D4">
-        <v>243622860</v>
+        <v>243667720</v>
       </c>
       <c r="E4">
         <v>0.85000000000000009</v>
@@ -831,8 +914,18 @@
       <c r="H4" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="5" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I4" s="2" t="s">
+        <v>17</v>
+      </c>
+      <c r="J4" s="2" t="s">
+        <v>18</v>
+      </c>
+      <c r="K4" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="5" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A5" t="s">
         <v>21</v>
       </c>
@@ -840,68 +933,88 @@
         <v>22</v>
       </c>
       <c r="C5" t="s">
+        <v>10</v>
+      </c>
+      <c r="D5">
+        <v>306304700</v>
+      </c>
+      <c r="E5">
+        <v>0.7</v>
+      </c>
+      <c r="F5">
+        <v>0.49583948982893</v>
+      </c>
+      <c r="G5" t="s">
+        <v>11</v>
+      </c>
+      <c r="H5" t="s">
+        <v>12</v>
+      </c>
+      <c r="I5" s="3" t="s">
         <v>23</v>
       </c>
-      <c r="D5">
+      <c r="J5" s="3" t="s">
+        <v>24</v>
+      </c>
+      <c r="K5" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="6" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A6" s="4" t="s">
+        <v>23</v>
+      </c>
+      <c r="B6" t="s">
+        <v>24</v>
+      </c>
+      <c r="C6" t="s">
+        <v>19</v>
+      </c>
+      <c r="D6">
+        <v>461509585</v>
+      </c>
+      <c r="E6">
+        <v>0.75</v>
+      </c>
+      <c r="F6">
+        <v>1</v>
+      </c>
+      <c r="G6" t="s">
+        <v>11</v>
+      </c>
+      <c r="H6" t="s">
+        <v>20</v>
+      </c>
+      <c r="I6" s="2" t="s">
+        <v>25</v>
+      </c>
+      <c r="J6" s="2" t="s">
+        <v>26</v>
+      </c>
+      <c r="K6" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="7" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A7" t="s">
+        <v>25</v>
+      </c>
+      <c r="B7" t="s">
+        <v>26</v>
+      </c>
+      <c r="C7" t="s">
+        <v>27</v>
+      </c>
+      <c r="D7">
         <v>450499200</v>
       </c>
-      <c r="E5">
-        <v>1</v>
-      </c>
-      <c r="F5">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G5" t="s">
-        <v>11</v>
-      </c>
-      <c r="H5" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="6" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A6" t="s">
-        <v>24</v>
-      </c>
-      <c r="B6" t="s">
-        <v>25</v>
-      </c>
-      <c r="C6" t="s">
-        <v>15</v>
-      </c>
-      <c r="D6">
-        <v>1445343300</v>
-      </c>
-      <c r="E6">
-        <v>1</v>
-      </c>
-      <c r="F6">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G6" t="s">
-        <v>11</v>
-      </c>
-      <c r="H6" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="7" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A7" t="s">
-        <v>26</v>
-      </c>
-      <c r="B7" t="s">
-        <v>27</v>
-      </c>
-      <c r="C7" t="s">
-        <v>19</v>
-      </c>
-      <c r="D7">
-        <v>75043514</v>
-      </c>
       <c r="E7">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F7">
-        <v>1</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G7" t="s">
         <v>11</v>
@@ -909,8 +1022,18 @@
       <c r="H7" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="8" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I7" s="3" t="s">
+        <v>28</v>
+      </c>
+      <c r="J7" s="3" t="s">
+        <v>29</v>
+      </c>
+      <c r="K7" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="8" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A8" t="s">
         <v>28</v>
       </c>
@@ -918,25 +1041,35 @@
         <v>29</v>
       </c>
       <c r="C8" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D8">
-        <v>2200619258</v>
+        <v>1550303800</v>
       </c>
       <c r="E8">
-        <v>0.85000000000000009</v>
+        <v>1</v>
       </c>
       <c r="F8">
-        <v>1</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G8" t="s">
         <v>11</v>
       </c>
       <c r="H8" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="9" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="I8" s="2" t="s">
+        <v>30</v>
+      </c>
+      <c r="J8" s="2" t="s">
+        <v>31</v>
+      </c>
+      <c r="K8" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="9" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A9" t="s">
         <v>30</v>
       </c>
@@ -944,25 +1077,35 @@
         <v>31</v>
       </c>
       <c r="C9" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D9">
-        <v>720076700</v>
+        <v>2201287926</v>
       </c>
       <c r="E9">
-        <v>1</v>
+        <v>0.85000000000000009</v>
       </c>
       <c r="F9">
-        <v>0.49351445259803001</v>
+        <v>1</v>
       </c>
       <c r="G9" t="s">
         <v>11</v>
       </c>
       <c r="H9" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="10" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I9" s="3" t="s">
+        <v>32</v>
+      </c>
+      <c r="J9" s="3" t="s">
+        <v>33</v>
+      </c>
+      <c r="K9" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="10" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A10" t="s">
         <v>32</v>
       </c>
@@ -970,25 +1113,35 @@
         <v>33</v>
       </c>
       <c r="C10" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D10">
-        <v>1130810671</v>
+        <v>289042420</v>
       </c>
       <c r="E10">
-        <v>0.95000000000000007</v>
+        <v>1</v>
       </c>
       <c r="F10">
-        <v>1</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G10" t="s">
         <v>11</v>
       </c>
       <c r="H10" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="11" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I10" s="2" t="s">
+        <v>34</v>
+      </c>
+      <c r="J10" s="2" t="s">
+        <v>35</v>
+      </c>
+      <c r="K10" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="11" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A11" t="s">
         <v>34</v>
       </c>
@@ -996,39 +1149,49 @@
         <v>35</v>
       </c>
       <c r="C11" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D11">
-        <v>453871520</v>
+        <v>145719350</v>
       </c>
       <c r="E11">
-        <v>0.75</v>
+        <v>1</v>
       </c>
       <c r="F11">
-        <v>1</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G11" t="s">
         <v>11</v>
       </c>
       <c r="H11" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="12" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I11" s="3" t="s">
+        <v>37</v>
+      </c>
+      <c r="J11" s="3" t="s">
+        <v>38</v>
+      </c>
+      <c r="K11" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="12" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A12" t="s">
-        <v>36</v>
+        <v>37</v>
       </c>
       <c r="B12" t="s">
-        <v>37</v>
+        <v>38</v>
       </c>
       <c r="C12" t="s">
         <v>19</v>
       </c>
       <c r="D12">
-        <v>677969188</v>
+        <v>118361220</v>
       </c>
       <c r="E12">
-        <v>0.8</v>
+        <v>0.4</v>
       </c>
       <c r="F12">
         <v>1</v>
@@ -1039,164 +1202,234 @@
       <c r="H12" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="13" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I12" s="2" t="s">
+        <v>39</v>
+      </c>
+      <c r="J12" s="2" t="s">
+        <v>40</v>
+      </c>
+      <c r="K12" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="13" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A13" t="s">
-        <v>38</v>
+        <v>39</v>
       </c>
       <c r="B13" t="s">
-        <v>39</v>
+        <v>40</v>
       </c>
       <c r="C13" t="s">
-        <v>40</v>
+        <v>15</v>
       </c>
       <c r="D13">
-        <v>201180500</v>
+        <v>722002700</v>
       </c>
       <c r="E13">
-        <v>0.9</v>
+        <v>1</v>
       </c>
       <c r="F13">
-        <v>0.49351445259803001</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G13" t="s">
         <v>11</v>
       </c>
       <c r="H13" t="s">
+        <v>16</v>
+      </c>
+      <c r="I13" s="3" t="s">
         <v>41</v>
       </c>
-    </row>
-    <row r="14" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J13" s="3" t="s">
+        <v>42</v>
+      </c>
+      <c r="K13" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="14" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A14" t="s">
+        <v>41</v>
+      </c>
+      <c r="B14" t="s">
         <v>42</v>
       </c>
-      <c r="B14" t="s">
+      <c r="C14" t="s">
+        <v>19</v>
+      </c>
+      <c r="D14">
+        <v>1130810671</v>
+      </c>
+      <c r="E14">
+        <v>0.95000000000000007</v>
+      </c>
+      <c r="F14">
+        <v>1</v>
+      </c>
+      <c r="G14" t="s">
+        <v>11</v>
+      </c>
+      <c r="H14" t="s">
+        <v>20</v>
+      </c>
+      <c r="I14" s="2" t="s">
         <v>43</v>
       </c>
-      <c r="C14" t="s">
-        <v>15</v>
-      </c>
-      <c r="D14">
-        <v>855700800</v>
-      </c>
-      <c r="E14">
-        <v>0.9</v>
-      </c>
-      <c r="F14">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G14" t="s">
-        <v>11</v>
-      </c>
-      <c r="H14" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="15" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="J14" s="2" t="s">
+        <v>44</v>
+      </c>
+      <c r="K14" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="15" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A15" t="s">
+        <v>43</v>
+      </c>
+      <c r="B15" t="s">
         <v>44</v>
-      </c>
-      <c r="B15" t="s">
-        <v>45</v>
       </c>
       <c r="C15" t="s">
         <v>19</v>
       </c>
       <c r="D15">
-        <v>3025902350</v>
+        <v>378957297</v>
       </c>
       <c r="E15">
+        <v>0.5</v>
+      </c>
+      <c r="F15">
+        <v>1</v>
+      </c>
+      <c r="G15" t="s">
+        <v>11</v>
+      </c>
+      <c r="H15" t="s">
+        <v>20</v>
+      </c>
+      <c r="I15" s="3" t="s">
+        <v>45</v>
+      </c>
+      <c r="J15" s="3" t="s">
+        <v>46</v>
+      </c>
+      <c r="K15" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="16" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A16" t="s">
+        <v>45</v>
+      </c>
+      <c r="B16" t="s">
+        <v>46</v>
+      </c>
+      <c r="C16" t="s">
+        <v>47</v>
+      </c>
+      <c r="D16">
+        <v>203856400</v>
+      </c>
+      <c r="E16">
+        <v>0.9</v>
+      </c>
+      <c r="F16">
+        <v>0.49583948982893</v>
+      </c>
+      <c r="G16" t="s">
+        <v>11</v>
+      </c>
+      <c r="H16" t="s">
+        <v>48</v>
+      </c>
+      <c r="I16" s="2" t="s">
+        <v>49</v>
+      </c>
+      <c r="J16" s="2" t="s">
+        <v>50</v>
+      </c>
+      <c r="K16" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="17" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A17" t="s">
+        <v>49</v>
+      </c>
+      <c r="B17" t="s">
+        <v>50</v>
+      </c>
+      <c r="C17" t="s">
+        <v>15</v>
+      </c>
+      <c r="D17">
+        <v>856208740</v>
+      </c>
+      <c r="E17">
+        <v>0.9</v>
+      </c>
+      <c r="F17">
+        <v>0.49583948982893</v>
+      </c>
+      <c r="G17" t="s">
+        <v>11</v>
+      </c>
+      <c r="H17" t="s">
+        <v>16</v>
+      </c>
+      <c r="I17" s="3" t="s">
+        <v>51</v>
+      </c>
+      <c r="J17" s="3" t="s">
+        <v>52</v>
+      </c>
+      <c r="K17" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="18" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A18" t="s">
+        <v>51</v>
+      </c>
+      <c r="B18" t="s">
+        <v>52</v>
+      </c>
+      <c r="C18" t="s">
+        <v>19</v>
+      </c>
+      <c r="D18">
+        <v>3041031027</v>
+      </c>
+      <c r="E18">
         <v>0.3</v>
       </c>
-      <c r="F15">
-        <v>1</v>
-      </c>
-      <c r="G15" t="s">
-        <v>11</v>
-      </c>
-      <c r="H15" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="16" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A16" t="s">
-        <v>46</v>
-      </c>
-      <c r="B16" t="s">
-        <v>47</v>
-      </c>
-      <c r="C16" t="s">
-        <v>19</v>
-      </c>
-      <c r="D16">
-        <v>679553991</v>
-      </c>
-      <c r="E16">
-        <v>0.95000000000000007</v>
-      </c>
-      <c r="F16">
-        <v>1</v>
-      </c>
-      <c r="G16" t="s">
-        <v>11</v>
-      </c>
-      <c r="H16" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="17" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A17" t="s">
-        <v>48</v>
-      </c>
-      <c r="B17" t="s">
-        <v>49</v>
-      </c>
-      <c r="C17" t="s">
-        <v>19</v>
-      </c>
-      <c r="D17">
-        <v>98000000</v>
-      </c>
-      <c r="E17">
-        <v>0.75</v>
-      </c>
-      <c r="F17">
-        <v>1</v>
-      </c>
-      <c r="G17" t="s">
-        <v>11</v>
-      </c>
-      <c r="H17" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="18" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A18" t="s">
-        <v>50</v>
-      </c>
-      <c r="B18" t="s">
-        <v>51</v>
-      </c>
-      <c r="C18" t="s">
-        <v>52</v>
-      </c>
-      <c r="D18">
-        <v>94944990</v>
-      </c>
-      <c r="E18">
-        <v>1</v>
-      </c>
       <c r="F18">
-        <v>0.49351445259803001</v>
+        <v>1</v>
       </c>
       <c r="G18" t="s">
         <v>11</v>
       </c>
       <c r="H18" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="19" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I18" s="2" t="s">
+        <v>53</v>
+      </c>
+      <c r="J18" s="2" t="s">
+        <v>54</v>
+      </c>
+      <c r="K18" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="19" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A19" t="s">
         <v>53</v>
       </c>
@@ -1204,25 +1437,35 @@
         <v>54</v>
       </c>
       <c r="C19" t="s">
-        <v>15</v>
+        <v>19</v>
       </c>
       <c r="D19">
-        <v>558145700</v>
+        <v>679553991</v>
       </c>
       <c r="E19">
-        <v>1</v>
+        <v>0.95000000000000007</v>
       </c>
       <c r="F19">
-        <v>0.49351445259803001</v>
+        <v>1</v>
       </c>
       <c r="G19" t="s">
         <v>11</v>
       </c>
       <c r="H19" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="20" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I19" s="3" t="s">
+        <v>55</v>
+      </c>
+      <c r="J19" s="3" t="s">
+        <v>56</v>
+      </c>
+      <c r="K19" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="20" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A20" t="s">
         <v>55</v>
       </c>
@@ -1230,25 +1473,35 @@
         <v>56</v>
       </c>
       <c r="C20" t="s">
-        <v>10</v>
+        <v>19</v>
       </c>
       <c r="D20">
-        <v>4145058000</v>
+        <v>98000000</v>
       </c>
       <c r="E20">
-        <v>1</v>
+        <v>0.75</v>
       </c>
       <c r="F20">
-        <v>0.49351445259803001</v>
+        <v>1</v>
       </c>
       <c r="G20" t="s">
         <v>11</v>
       </c>
       <c r="H20" t="s">
-        <v>12</v>
-      </c>
-    </row>
-    <row r="21" spans="1:8" x14ac:dyDescent="0.25">
+        <v>20</v>
+      </c>
+      <c r="I20" s="2" t="s">
+        <v>57</v>
+      </c>
+      <c r="J20" s="2" t="s">
+        <v>58</v>
+      </c>
+      <c r="K20" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="21" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A21" t="s">
         <v>57</v>
       </c>
@@ -1256,25 +1509,35 @@
         <v>58</v>
       </c>
       <c r="C21" t="s">
-        <v>19</v>
+        <v>36</v>
       </c>
       <c r="D21">
-        <v>105569412</v>
+        <v>96488190</v>
       </c>
       <c r="E21">
-        <v>0.3</v>
+        <v>1</v>
       </c>
       <c r="F21">
-        <v>1</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G21" t="s">
         <v>11</v>
       </c>
       <c r="H21" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="22" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I21" s="3" t="s">
+        <v>107</v>
+      </c>
+      <c r="J21" s="3" t="s">
+        <v>104</v>
+      </c>
+      <c r="K21" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="22" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A22" t="s">
         <v>59</v>
       </c>
@@ -1282,25 +1545,35 @@
         <v>60</v>
       </c>
       <c r="C22" t="s">
-        <v>19</v>
+        <v>15</v>
       </c>
       <c r="D22">
-        <v>123420778</v>
+        <v>555158900</v>
       </c>
       <c r="E22">
-        <v>0.60000000000000009</v>
+        <v>1</v>
       </c>
       <c r="F22">
-        <v>1</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G22" t="s">
         <v>11</v>
       </c>
       <c r="H22" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="23" spans="1:8" x14ac:dyDescent="0.25">
+        <v>16</v>
+      </c>
+      <c r="I22" s="2" t="s">
+        <v>59</v>
+      </c>
+      <c r="J22" s="2" t="s">
+        <v>60</v>
+      </c>
+      <c r="K22" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="23" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A23" t="s">
         <v>61</v>
       </c>
@@ -1311,13 +1584,13 @@
         <v>10</v>
       </c>
       <c r="D23">
-        <v>1838668600</v>
+        <v>4145099600</v>
       </c>
       <c r="E23">
-        <v>0.85</v>
+        <v>1</v>
       </c>
       <c r="F23">
-        <v>0.49351445259803001</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G23" t="s">
         <v>11</v>
@@ -1325,8 +1598,18 @@
       <c r="H23" t="s">
         <v>12</v>
       </c>
-    </row>
-    <row r="24" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I23" s="3" t="s">
+        <v>61</v>
+      </c>
+      <c r="J23" s="3" t="s">
+        <v>62</v>
+      </c>
+      <c r="K23" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="24" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A24" t="s">
         <v>63</v>
       </c>
@@ -1337,10 +1620,10 @@
         <v>19</v>
       </c>
       <c r="D24">
-        <v>534955898</v>
+        <v>105569412</v>
       </c>
       <c r="E24">
-        <v>0.45</v>
+        <v>0.3</v>
       </c>
       <c r="F24">
         <v>1</v>
@@ -1351,8 +1634,18 @@
       <c r="H24" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="25" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I24" s="2" t="s">
+        <v>63</v>
+      </c>
+      <c r="J24" s="2" t="s">
+        <v>64</v>
+      </c>
+      <c r="K24" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="25" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A25" t="s">
         <v>65</v>
       </c>
@@ -1360,25 +1653,35 @@
         <v>66</v>
       </c>
       <c r="C25" t="s">
-        <v>19</v>
+        <v>10</v>
       </c>
       <c r="D25">
-        <v>500141700</v>
+        <v>1813468600</v>
       </c>
       <c r="E25">
-        <v>0.5</v>
+        <v>0.85</v>
       </c>
       <c r="F25">
-        <v>0.94644311401342995</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G25" t="s">
         <v>11</v>
       </c>
       <c r="H25" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="26" spans="1:8" x14ac:dyDescent="0.25">
+        <v>12</v>
+      </c>
+      <c r="I25" s="3" t="s">
+        <v>65</v>
+      </c>
+      <c r="J25" s="3" t="s">
+        <v>66</v>
+      </c>
+      <c r="K25" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="26" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A26" t="s">
         <v>67</v>
       </c>
@@ -1386,39 +1689,49 @@
         <v>68</v>
       </c>
       <c r="C26" t="s">
+        <v>19</v>
+      </c>
+      <c r="D26">
+        <v>534311946</v>
+      </c>
+      <c r="E26">
+        <v>0.45</v>
+      </c>
+      <c r="F26">
+        <v>1</v>
+      </c>
+      <c r="G26" t="s">
+        <v>11</v>
+      </c>
+      <c r="H26" t="s">
+        <v>20</v>
+      </c>
+      <c r="I26" s="2" t="s">
+        <v>67</v>
+      </c>
+      <c r="J26" s="2" t="s">
+        <v>68</v>
+      </c>
+      <c r="K26" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="27" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A27" t="s">
         <v>69</v>
       </c>
-      <c r="D26">
-        <v>129242250</v>
-      </c>
-      <c r="E26">
-        <v>1</v>
-      </c>
-      <c r="F26">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G26" t="s">
-        <v>11</v>
-      </c>
-      <c r="H26" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="27" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A27" t="s">
+      <c r="B27" t="s">
         <v>70</v>
-      </c>
-      <c r="B27" t="s">
-        <v>71</v>
       </c>
       <c r="C27" t="s">
         <v>19</v>
       </c>
       <c r="D27">
-        <v>714958226</v>
+        <v>500141700</v>
       </c>
       <c r="E27">
-        <v>1</v>
+        <v>0.5</v>
       </c>
       <c r="F27">
         <v>1</v>
@@ -1429,39 +1742,59 @@
       <c r="H27" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="28" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I27" s="3" t="s">
+        <v>69</v>
+      </c>
+      <c r="J27" s="3" t="s">
+        <v>70</v>
+      </c>
+      <c r="K27" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="28" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A28" t="s">
+        <v>71</v>
+      </c>
+      <c r="B28" t="s">
         <v>72</v>
       </c>
-      <c r="B28" t="s">
+      <c r="C28" t="s">
         <v>73</v>
       </c>
-      <c r="C28" t="s">
+      <c r="D28">
+        <v>129242250</v>
+      </c>
+      <c r="E28">
+        <v>1</v>
+      </c>
+      <c r="F28">
+        <v>0.49583948982893</v>
+      </c>
+      <c r="G28" t="s">
+        <v>11</v>
+      </c>
+      <c r="H28" t="s">
+        <v>20</v>
+      </c>
+      <c r="I28" s="2" t="s">
+        <v>71</v>
+      </c>
+      <c r="J28" s="2" t="s">
+        <v>72</v>
+      </c>
+      <c r="K28" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="29" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A29" t="s">
         <v>74</v>
       </c>
-      <c r="D28">
-        <v>2620000000</v>
-      </c>
-      <c r="E28">
-        <v>1</v>
-      </c>
-      <c r="F28">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G28" t="s">
-        <v>11</v>
-      </c>
-      <c r="H28" t="s">
+      <c r="B29" t="s">
         <v>75</v>
-      </c>
-    </row>
-    <row r="29" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A29" t="s">
-        <v>76</v>
-      </c>
-      <c r="B29" t="s">
-        <v>77</v>
       </c>
       <c r="C29" t="s">
         <v>19</v>
@@ -1481,39 +1814,59 @@
       <c r="H29" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="30" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I29" s="3" t="s">
+        <v>108</v>
+      </c>
+      <c r="J29" s="3" t="s">
+        <v>105</v>
+      </c>
+      <c r="K29" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="30" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A30" t="s">
+        <v>76</v>
+      </c>
+      <c r="B30" t="s">
+        <v>77</v>
+      </c>
+      <c r="C30" t="s">
         <v>78</v>
       </c>
-      <c r="B30" t="s">
+      <c r="D30">
+        <v>5613496600</v>
+      </c>
+      <c r="E30">
+        <v>0.95</v>
+      </c>
+      <c r="F30">
+        <v>0.49583948982893</v>
+      </c>
+      <c r="G30" t="s">
+        <v>11</v>
+      </c>
+      <c r="H30" t="s">
+        <v>20</v>
+      </c>
+      <c r="I30" s="2" t="s">
+        <v>74</v>
+      </c>
+      <c r="J30" s="2" t="s">
+        <v>75</v>
+      </c>
+      <c r="K30" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="31" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A31" t="s">
         <v>79</v>
       </c>
-      <c r="C30" t="s">
-        <v>19</v>
-      </c>
-      <c r="D30">
-        <v>253328748</v>
-      </c>
-      <c r="E30">
-        <v>0.8</v>
-      </c>
-      <c r="F30">
-        <v>1</v>
-      </c>
-      <c r="G30" t="s">
-        <v>11</v>
-      </c>
-      <c r="H30" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="31" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A31" t="s">
+      <c r="B31" t="s">
         <v>80</v>
-      </c>
-      <c r="B31" t="s">
-        <v>81</v>
       </c>
       <c r="C31" t="s">
         <v>19</v>
@@ -1533,16 +1886,26 @@
       <c r="H31" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="32" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I31" s="3" t="s">
+        <v>76</v>
+      </c>
+      <c r="J31" s="3" t="s">
+        <v>77</v>
+      </c>
+      <c r="K31" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="32" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A32" t="s">
+        <v>81</v>
+      </c>
+      <c r="B32" t="s">
         <v>82</v>
       </c>
-      <c r="B32" t="s">
+      <c r="C32" t="s">
         <v>83</v>
-      </c>
-      <c r="C32" t="s">
-        <v>84</v>
       </c>
       <c r="D32">
         <v>180869312</v>
@@ -1551,7 +1914,7 @@
         <v>0.5</v>
       </c>
       <c r="F32">
-        <v>0.49351445259803001</v>
+        <v>0.49583948982893</v>
       </c>
       <c r="G32" t="s">
         <v>11</v>
@@ -1559,19 +1922,29 @@
       <c r="H32" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="33" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I32" s="2" t="s">
+        <v>79</v>
+      </c>
+      <c r="J32" s="2" t="s">
+        <v>80</v>
+      </c>
+      <c r="K32" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="33" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A33" t="s">
+        <v>84</v>
+      </c>
+      <c r="B33" t="s">
         <v>85</v>
-      </c>
-      <c r="B33" t="s">
-        <v>86</v>
       </c>
       <c r="C33" t="s">
         <v>19</v>
       </c>
       <c r="D33">
-        <v>301735000</v>
+        <v>295722284</v>
       </c>
       <c r="E33">
         <v>0.70000000000000007</v>
@@ -1585,216 +1958,428 @@
       <c r="H33" t="s">
         <v>20</v>
       </c>
-    </row>
-    <row r="34" spans="1:8" x14ac:dyDescent="0.25">
+      <c r="I33" s="3" t="s">
+        <v>81</v>
+      </c>
+      <c r="J33" s="3" t="s">
+        <v>82</v>
+      </c>
+      <c r="K33" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="34" spans="1:11" x14ac:dyDescent="0.25">
       <c r="A34" t="s">
+        <v>86</v>
+      </c>
+      <c r="B34" t="s">
         <v>87</v>
-      </c>
-      <c r="B34" t="s">
-        <v>88</v>
       </c>
       <c r="C34" t="s">
         <v>19</v>
       </c>
       <c r="D34">
+        <v>298233069</v>
+      </c>
+      <c r="E34">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="F34">
+        <v>1</v>
+      </c>
+      <c r="G34" t="s">
+        <v>11</v>
+      </c>
+      <c r="H34" t="s">
+        <v>20</v>
+      </c>
+      <c r="I34" s="2" t="s">
+        <v>84</v>
+      </c>
+      <c r="J34" s="2" t="s">
+        <v>85</v>
+      </c>
+      <c r="K34" t="b">
+        <f t="shared" si="0"/>
+        <v>0</v>
+      </c>
+    </row>
+    <row r="35" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A35" t="s">
+        <v>88</v>
+      </c>
+      <c r="B35" t="s">
+        <v>89</v>
+      </c>
+      <c r="C35" t="s">
+        <v>19</v>
+      </c>
+      <c r="D35">
         <v>504005802</v>
       </c>
-      <c r="E34">
+      <c r="E35">
         <v>0.9</v>
       </c>
-      <c r="F34">
-        <v>1</v>
-      </c>
-      <c r="G34" t="s">
-        <v>11</v>
-      </c>
-      <c r="H34" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="35" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A35" t="s">
+      <c r="F35">
+        <v>1</v>
+      </c>
+      <c r="G35" t="s">
+        <v>11</v>
+      </c>
+      <c r="H35" t="s">
+        <v>20</v>
+      </c>
+      <c r="I35" s="3" t="s">
+        <v>88</v>
+      </c>
+      <c r="J35" s="3" t="s">
         <v>89</v>
       </c>
-      <c r="B35" t="s">
+      <c r="K35" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="36" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A36" t="s">
         <v>90</v>
       </c>
-      <c r="C35" t="s">
+      <c r="B36" t="s">
         <v>91</v>
       </c>
-      <c r="D35">
-        <v>546454160</v>
-      </c>
-      <c r="E35">
-        <v>0.85</v>
-      </c>
-      <c r="F35">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G35" t="s">
-        <v>11</v>
-      </c>
-      <c r="H35" t="s">
+      <c r="C36" t="s">
+        <v>19</v>
+      </c>
+      <c r="D36">
+        <v>1268922721</v>
+      </c>
+      <c r="E36">
+        <v>0.9</v>
+      </c>
+      <c r="F36">
+        <v>1</v>
+      </c>
+      <c r="G36" t="s">
+        <v>11</v>
+      </c>
+      <c r="H36" t="s">
+        <v>20</v>
+      </c>
+      <c r="I36" s="2" t="s">
+        <v>90</v>
+      </c>
+      <c r="J36" s="2" t="s">
+        <v>91</v>
+      </c>
+      <c r="K36" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="37" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A37" t="s">
         <v>92</v>
       </c>
-    </row>
-    <row r="36" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A36" t="s">
+      <c r="B37" t="s">
         <v>93</v>
       </c>
-      <c r="B36" t="s">
+      <c r="C37" t="s">
+        <v>73</v>
+      </c>
+      <c r="D37">
+        <v>800000000</v>
+      </c>
+      <c r="E37">
+        <v>0.95</v>
+      </c>
+      <c r="F37">
+        <v>0.49583948982893</v>
+      </c>
+      <c r="G37" t="s">
+        <v>11</v>
+      </c>
+      <c r="H37" t="s">
+        <v>20</v>
+      </c>
+      <c r="I37" s="3" t="s">
+        <v>92</v>
+      </c>
+      <c r="J37" s="3" t="s">
+        <v>93</v>
+      </c>
+      <c r="K37" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="38" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A38" t="s">
         <v>94</v>
       </c>
-      <c r="C36" t="s">
-        <v>69</v>
-      </c>
-      <c r="D36">
-        <v>800000000</v>
-      </c>
-      <c r="E36">
-        <v>0.95</v>
-      </c>
-      <c r="F36">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G36" t="s">
-        <v>11</v>
-      </c>
-      <c r="H36" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="37" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A37" t="s">
+      <c r="B38" t="s">
         <v>95</v>
       </c>
-      <c r="B37" t="s">
+      <c r="C38" t="s">
+        <v>19</v>
+      </c>
+      <c r="D38">
+        <v>911281920</v>
+      </c>
+      <c r="E38">
+        <v>0.70000000000000007</v>
+      </c>
+      <c r="F38">
+        <v>1</v>
+      </c>
+      <c r="G38" t="s">
+        <v>11</v>
+      </c>
+      <c r="H38" t="s">
+        <v>20</v>
+      </c>
+      <c r="I38" s="2" t="s">
+        <v>94</v>
+      </c>
+      <c r="J38" s="2" t="s">
+        <v>95</v>
+      </c>
+      <c r="K38" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="39" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A39" t="s">
         <v>96</v>
       </c>
-      <c r="C37" t="s">
-        <v>74</v>
-      </c>
-      <c r="D37">
-        <v>28727518</v>
-      </c>
-      <c r="E37">
-        <v>1</v>
-      </c>
-      <c r="F37">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G37" t="s">
-        <v>11</v>
-      </c>
-      <c r="H37" t="s">
-        <v>75</v>
-      </c>
-    </row>
-    <row r="38" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A38" t="s">
+      <c r="B39" t="s">
         <v>97</v>
       </c>
-      <c r="B38" t="s">
+      <c r="C39" t="s">
+        <v>15</v>
+      </c>
+      <c r="D39">
+        <v>382500270</v>
+      </c>
+      <c r="E39">
+        <v>1</v>
+      </c>
+      <c r="F39">
+        <v>0.49583948982893</v>
+      </c>
+      <c r="G39" t="s">
+        <v>11</v>
+      </c>
+      <c r="H39" t="s">
+        <v>16</v>
+      </c>
+      <c r="I39" s="3" t="s">
+        <v>96</v>
+      </c>
+      <c r="J39" s="3" t="s">
+        <v>97</v>
+      </c>
+      <c r="K39" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="40" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A40" t="s">
         <v>98</v>
       </c>
-      <c r="C38" t="s">
-        <v>15</v>
-      </c>
-      <c r="D38">
-        <v>381995570</v>
-      </c>
-      <c r="E38">
-        <v>1</v>
-      </c>
-      <c r="F38">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G38" t="s">
-        <v>11</v>
-      </c>
-      <c r="H38" t="s">
-        <v>16</v>
-      </c>
-    </row>
-    <row r="39" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A39" t="s">
+      <c r="B40" t="s">
         <v>99</v>
       </c>
-      <c r="B39" t="s">
+      <c r="C40" t="s">
         <v>100</v>
       </c>
-      <c r="C39" t="s">
+      <c r="D40">
+        <v>15794987000</v>
+      </c>
+      <c r="E40">
+        <v>0.75</v>
+      </c>
+      <c r="F40">
+        <v>0.49583948982893</v>
+      </c>
+      <c r="G40" t="s">
+        <v>11</v>
+      </c>
+      <c r="H40" t="s">
         <v>101</v>
       </c>
-      <c r="D39">
-        <v>15794987000</v>
-      </c>
-      <c r="E39">
-        <v>0.8</v>
-      </c>
-      <c r="F39">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G39" t="s">
-        <v>11</v>
-      </c>
-      <c r="H39" t="s">
+      <c r="I40" s="2" t="s">
+        <v>98</v>
+      </c>
+      <c r="J40" s="2" t="s">
+        <v>99</v>
+      </c>
+      <c r="K40" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="41" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="A41" t="s">
         <v>102</v>
       </c>
-    </row>
-    <row r="40" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A40" t="s">
+      <c r="B41" t="s">
         <v>103</v>
       </c>
-      <c r="B40" t="s">
-        <v>104</v>
-      </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>19</v>
       </c>
-      <c r="D40">
-        <v>588519218</v>
-      </c>
-      <c r="E40">
+      <c r="D41">
+        <v>589895166</v>
+      </c>
+      <c r="E41">
         <v>0.9</v>
       </c>
-      <c r="F40">
-        <v>1</v>
-      </c>
-      <c r="G40" t="s">
-        <v>11</v>
-      </c>
-      <c r="H40" t="s">
-        <v>20</v>
-      </c>
-    </row>
-    <row r="41" spans="1:8" x14ac:dyDescent="0.25">
-      <c r="A41" t="s">
-        <v>105</v>
-      </c>
-      <c r="B41" t="s">
+      <c r="F41">
+        <v>1</v>
+      </c>
+      <c r="G41" t="s">
+        <v>11</v>
+      </c>
+      <c r="H41" t="s">
+        <v>20</v>
+      </c>
+      <c r="I41" s="3" t="s">
+        <v>102</v>
+      </c>
+      <c r="J41" s="3" t="s">
+        <v>103</v>
+      </c>
+      <c r="K41" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="42" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I42" s="2" t="s">
         <v>106</v>
       </c>
-      <c r="C41" t="s">
-        <v>15</v>
-      </c>
-      <c r="D41">
-        <v>203652370</v>
-      </c>
-      <c r="E41">
-        <v>1</v>
-      </c>
-      <c r="F41">
-        <v>0.49351445259803001</v>
-      </c>
-      <c r="G41" t="s">
-        <v>11</v>
-      </c>
-      <c r="H41" t="s">
-        <v>16</v>
+      <c r="J42" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K42" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="43" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I43" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J43" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K43" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="44" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I44" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J44" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K44" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="45" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J45" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K45" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="46" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I46" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J46" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K46" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="47" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I47" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J47" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K47" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="48" spans="1:11" x14ac:dyDescent="0.25">
+      <c r="I48" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J48" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="K48" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="49" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I49" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J49" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="K49" t="b">
+        <f t="shared" si="0"/>
+        <v>1</v>
+      </c>
+    </row>
+    <row r="50" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I50" s="2" t="s">
+        <v>106</v>
+      </c>
+      <c r="J50" s="2" t="s">
+        <v>106</v>
+      </c>
+    </row>
+    <row r="51" spans="9:11" x14ac:dyDescent="0.25">
+      <c r="I51" s="3" t="s">
+        <v>106</v>
+      </c>
+      <c r="J51" s="3" t="s">
+        <v>106</v>
       </c>
     </row>
   </sheetData>
+  <conditionalFormatting sqref="J2:J51">
+    <cfRule type="cellIs" dxfId="1" priority="2" operator="equal">
+      <formula>"ADD NEW RECORD"</formula>
+    </cfRule>
+  </conditionalFormatting>
+  <conditionalFormatting sqref="I2:I51">
+    <cfRule type="cellIs" dxfId="0" priority="1" operator="equal">
+      <formula>"ADD NEW RECORD"</formula>
+    </cfRule>
+  </conditionalFormatting>
   <pageMargins left="0.75" right="0.75" top="1" bottom="1" header="0.5" footer="0.5"/>
   <headerFooter>
     <oddFooter>&amp;C_x000D_&amp;1#&amp;"Calibri"&amp;10&amp;KFFEF00 PRIVATE</oddFooter>

</xml_diff>